<commit_message>
fixing upload process file algorthim
</commit_message>
<xml_diff>
--- a/admin/public/excel/en/2019/Average-perfomance.xlsx
+++ b/admin/public/excel/en/2019/Average-perfomance.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olive\Desktop\INDEX1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olive\Desktop\INDEX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16905" tabRatio="766"/>
   </bookViews>
   <sheets>
-    <sheet name="Index by Country" sheetId="3" r:id="rId1"/>
+    <sheet name="Index by Country" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="150001"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Index by Country'!$A$1:$S$55</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -359,58 +359,58 @@
     <t>ZWE</t>
   </si>
   <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>sdg17</t>
+  </si>
+  <si>
+    <t>sdg16</t>
+  </si>
+  <si>
+    <t>sdg15</t>
+  </si>
+  <si>
+    <t>sdg14</t>
+  </si>
+  <si>
+    <t>sdg13</t>
+  </si>
+  <si>
+    <t>sdg12</t>
+  </si>
+  <si>
+    <t>sdg11</t>
+  </si>
+  <si>
+    <t>sdg10</t>
+  </si>
+  <si>
+    <t>sdg9</t>
+  </si>
+  <si>
+    <t>sdg8</t>
+  </si>
+  <si>
+    <t>sdg7</t>
+  </si>
+  <si>
+    <t>sdg6</t>
+  </si>
+  <si>
+    <t>sdg5</t>
+  </si>
+  <si>
+    <t>sdg4</t>
+  </si>
+  <si>
+    <t>sdg3</t>
+  </si>
+  <si>
+    <t>sdg2</t>
+  </si>
+  <si>
     <t>sdg1</t>
-  </si>
-  <si>
-    <t>sdg2</t>
-  </si>
-  <si>
-    <t>sdg3</t>
-  </si>
-  <si>
-    <t>sdg4</t>
-  </si>
-  <si>
-    <t>sdg5</t>
-  </si>
-  <si>
-    <t>sdg6</t>
-  </si>
-  <si>
-    <t>sdg7</t>
-  </si>
-  <si>
-    <t>sdg8</t>
-  </si>
-  <si>
-    <t>sdg9</t>
-  </si>
-  <si>
-    <t>sdg10</t>
-  </si>
-  <si>
-    <t>sdg11</t>
-  </si>
-  <si>
-    <t>sdg12</t>
-  </si>
-  <si>
-    <t>sdg13</t>
-  </si>
-  <si>
-    <t>sdg14</t>
-  </si>
-  <si>
-    <t>sdg15</t>
-  </si>
-  <si>
-    <t>sdg16</t>
-  </si>
-  <si>
-    <t>sdg17</t>
-  </si>
-  <si>
-    <t>Eswatini</t>
   </si>
 </sst>
 </file>
@@ -477,38 +477,7 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -519,23 +488,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Old error data"/>
-      <sheetName val="NEW CORRECT DATA"/>
-      <sheetName val="Feuil2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -837,15 +789,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="37.5">
       <c r="A1" s="1" t="s">
@@ -855,55 +803,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -950,7 +898,7 @@
         <v>71.801632964147643</v>
       </c>
       <c r="O2">
-        <v>90.640357431246002</v>
+        <v>94.277237098703324</v>
       </c>
       <c r="P2">
         <v>43.112964694341272</v>
@@ -1009,7 +957,7 @@
         <v>83.225583364531047</v>
       </c>
       <c r="O3">
-        <v>89.481757945732568</v>
+        <v>90.89123150835124</v>
       </c>
       <c r="P3">
         <v>43.372129001890677</v>
@@ -1068,7 +1016,7 @@
         <v>95.702531626786666</v>
       </c>
       <c r="O4">
-        <v>96.639733223590397</v>
+        <v>97.349934414483229</v>
       </c>
       <c r="P4">
         <v>34.436831772338145</v>
@@ -1127,10 +1075,10 @@
         <v>63.400425476434101</v>
       </c>
       <c r="O5">
-        <v>68.19822136667392</v>
+        <v>71.507731105089135</v>
       </c>
       <c r="P5">
-        <v>55.790837233776934</v>
+        <v>55.790837233776948</v>
       </c>
       <c r="Q5">
         <v>78.137183349953546</v>
@@ -1186,10 +1134,10 @@
         <v>88.928411230908424</v>
       </c>
       <c r="O6">
-        <v>90.646270976760604</v>
+        <v>90.7871334290313</v>
       </c>
       <c r="P6">
-        <v>44.27088423266283</v>
+        <v>44.270884232662816</v>
       </c>
       <c r="Q6">
         <v>88.436631809333733</v>
@@ -1245,10 +1193,10 @@
         <v>95.875436052358396</v>
       </c>
       <c r="O7">
-        <v>99.302661089336254</v>
+        <v>99.346061505243114</v>
       </c>
       <c r="P7">
-        <v>38.618197517357046</v>
+        <v>38.618197517357054</v>
       </c>
       <c r="Q7">
         <v>79.341241564991563</v>
@@ -1304,7 +1252,7 @@
         <v>91.795760048341279</v>
       </c>
       <c r="O8">
-        <v>88.527909528702352</v>
+        <v>89.87492051718398</v>
       </c>
       <c r="P8">
         <v>40.430588287052565</v>
@@ -1363,7 +1311,7 @@
         <v>85.969446577224019</v>
       </c>
       <c r="O9">
-        <v>97.348339140348543</v>
+        <v>97.901885747456134</v>
       </c>
       <c r="P9">
         <v>35.615336132552279</v>
@@ -1422,7 +1370,7 @@
         <v>96.143286838560698</v>
       </c>
       <c r="O10">
-        <v>99.296732725784608</v>
+        <v>99.383745132147595</v>
       </c>
       <c r="P10">
         <v>47.139632909115051</v>
@@ -1481,7 +1429,7 @@
         <v>82.417308592282538</v>
       </c>
       <c r="O11">
-        <v>76.226842402121108</v>
+        <v>76.324158823245057</v>
       </c>
       <c r="P11">
         <v>47.139632909115051</v>
@@ -1540,7 +1488,7 @@
         <v>83.88688097367455</v>
       </c>
       <c r="O12">
-        <v>97.09725139451551</v>
+        <v>97.388939703791792</v>
       </c>
       <c r="P12">
         <v>22.183787759591162</v>
@@ -1599,7 +1547,7 @@
         <v>81.539858809579769</v>
       </c>
       <c r="O13">
-        <v>99.155843994441113</v>
+        <v>99.224616830973602</v>
       </c>
       <c r="P13">
         <v>8.0828121936274488</v>
@@ -1658,7 +1606,7 @@
         <v>81.56486358681255</v>
       </c>
       <c r="O14">
-        <v>94.428262962377332</v>
+        <v>95.199296525221101</v>
       </c>
       <c r="P14">
         <v>44.325295619065969</v>
@@ -1717,7 +1665,7 @@
         <v>87.53850595568025</v>
       </c>
       <c r="O15">
-        <v>98.994826249109678</v>
+        <v>99.43286567840731</v>
       </c>
       <c r="P15">
         <v>38.381434583477578</v>
@@ -1776,7 +1724,7 @@
         <v>98.095002004002893</v>
       </c>
       <c r="O16">
-        <v>90.279090312197994</v>
+        <v>90.937300482654692</v>
       </c>
       <c r="P16">
         <v>17.313892174369744</v>
@@ -1835,7 +1783,7 @@
         <v>73.270711658613763</v>
       </c>
       <c r="O17">
-        <v>95.819883331048544</v>
+        <v>97.8262138641538</v>
       </c>
       <c r="P17">
         <v>51.802706724584837</v>
@@ -1894,7 +1842,7 @@
         <v>71.323545214278113</v>
       </c>
       <c r="O18">
-        <v>54.679408108924733</v>
+        <v>77.339704054462359</v>
       </c>
       <c r="P18">
         <v>79.649880701669986</v>
@@ -1953,7 +1901,7 @@
         <v>77.004054415675597</v>
       </c>
       <c r="O19">
-        <v>98.976987929632074</v>
+        <v>99.143335120982314</v>
       </c>
       <c r="P19">
         <v>34.890801987916305</v>
@@ -1970,1670 +1918,1670 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C20">
-        <v>42.505793547706567</v>
+        <v>58.878940348399233</v>
       </c>
       <c r="D20">
-        <v>51.35001496993317</v>
+        <v>41.42329893936968</v>
       </c>
       <c r="E20">
-        <v>47.600861428392861</v>
+        <v>49.050752556127925</v>
       </c>
       <c r="F20">
-        <v>55.489767445624615</v>
+        <v>27.500983583092498</v>
       </c>
       <c r="G20">
-        <v>67.415641516136859</v>
+        <v>54.456706441599941</v>
       </c>
       <c r="H20">
-        <v>56.082005554379784</v>
+        <v>39.431877035585558</v>
       </c>
       <c r="I20">
-        <v>60.494537993584082</v>
+        <v>58.701315306830409</v>
       </c>
       <c r="J20">
-        <v>43.100343723833078</v>
+        <v>70.951536519923508</v>
       </c>
       <c r="K20">
-        <v>22.581650414461411</v>
+        <v>18.897698816212614</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>56.161971830985905</v>
       </c>
       <c r="M20">
-        <v>62.009661256175399</v>
+        <v>45.423392425579131</v>
       </c>
       <c r="N20">
-        <v>90.880649533926444</v>
+        <v>85.653638939033712</v>
       </c>
       <c r="O20">
-        <v>51.725320473881695</v>
+        <v>95.710345785108444</v>
       </c>
       <c r="P20">
-        <v>55.790837233776934</v>
+        <v>38.618197517357054</v>
       </c>
       <c r="Q20">
-        <v>63.345406887574399</v>
+        <v>66.82805469285141</v>
       </c>
       <c r="R20">
-        <v>51.460916515610414</v>
+        <v>49.692570491074989</v>
       </c>
       <c r="S20">
-        <v>67.233172079337876</v>
+        <v>47.319495682291254</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>58.878940348399233</v>
+        <v>71.92717273411354</v>
       </c>
       <c r="D21">
-        <v>41.42329893936968</v>
+        <v>54.628018737530823</v>
       </c>
       <c r="E21">
-        <v>49.050752556127925</v>
+        <v>48.305445883848037</v>
       </c>
       <c r="F21">
-        <v>27.500983583092498</v>
+        <v>66.575296825822008</v>
       </c>
       <c r="G21">
-        <v>54.456706441599941</v>
+        <v>54.03888080276392</v>
       </c>
       <c r="H21">
-        <v>39.431877035585558</v>
+        <v>61.692400215825955</v>
       </c>
       <c r="I21">
-        <v>58.701315306830409</v>
+        <v>85.71622950337111</v>
       </c>
       <c r="J21">
-        <v>70.951536519923508</v>
+        <v>55.489150162527757</v>
       </c>
       <c r="K21">
-        <v>18.897698816212614</v>
+        <v>36.960192060428845</v>
       </c>
       <c r="L21">
-        <v>56.161971830985905</v>
+        <v>36.605709002051555</v>
       </c>
       <c r="M21">
-        <v>45.423392425579131</v>
+        <v>40.511692585512648</v>
       </c>
       <c r="N21">
-        <v>85.653638939033712</v>
+        <v>71.852810177179748</v>
       </c>
       <c r="O21">
-        <v>95.596005010436784</v>
+        <v>94.661230934472428</v>
       </c>
       <c r="P21">
-        <v>38.618197517357046</v>
+        <v>68.483481947063211</v>
       </c>
       <c r="Q21">
-        <v>66.82805469285141</v>
+        <v>83.456310812352655</v>
       </c>
       <c r="R21">
-        <v>49.692570491074989</v>
+        <v>58.270168246704387</v>
       </c>
       <c r="S21">
-        <v>47.319495682291254</v>
+        <v>20.229404396039588</v>
       </c>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>71.92717273411354</v>
+        <v>31.242757934408004</v>
       </c>
       <c r="D22">
-        <v>54.628018737530823</v>
+        <v>40.84148597110628</v>
       </c>
       <c r="E22">
-        <v>48.305445883848037</v>
+        <v>44.571232273463622</v>
       </c>
       <c r="F22">
-        <v>66.575296825822008</v>
+        <v>36.904297401408833</v>
       </c>
       <c r="G22">
-        <v>54.03888080276392</v>
+        <v>32.467797984297533</v>
       </c>
       <c r="H22">
-        <v>61.692400215825955</v>
+        <v>59.973073512003523</v>
       </c>
       <c r="I22">
-        <v>85.71622950337111</v>
+        <v>32.752974398465732</v>
       </c>
       <c r="J22">
-        <v>55.489150162527757</v>
+        <v>55.089442768915461</v>
       </c>
       <c r="K22">
-        <v>36.960192060428845</v>
+        <v>17.952393799359559</v>
       </c>
       <c r="L22">
-        <v>36.605709002051555</v>
+        <v>53.065767019567346</v>
       </c>
       <c r="M22">
-        <v>40.511692585512648</v>
+        <v>48.479877426832999</v>
       </c>
       <c r="N22">
-        <v>71.852810177179748</v>
+        <v>95.342791521874872</v>
       </c>
       <c r="O22">
-        <v>89.32246186894487</v>
+        <v>93.52786039900306</v>
       </c>
       <c r="P22">
-        <v>68.483481947063211</v>
+        <v>45.936663233238519</v>
       </c>
       <c r="Q22">
-        <v>83.456310812352655</v>
+        <v>74.913103523916064</v>
       </c>
       <c r="R22">
-        <v>58.270168246704387</v>
+        <v>60.466517336358265</v>
       </c>
       <c r="S22">
-        <v>20.229404396039588</v>
+        <v>58.983703421804741</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23">
-        <v>31.242757934408004</v>
+        <v>77.133358060568455</v>
       </c>
       <c r="D23">
-        <v>40.84148597110628</v>
+        <v>55.774369750390484</v>
       </c>
       <c r="E23">
-        <v>44.571232273463622</v>
+        <v>53.247988411637131</v>
       </c>
       <c r="F23">
-        <v>36.904297401408833</v>
+        <v>63.65355531565524</v>
       </c>
       <c r="G23">
-        <v>32.467797984297533</v>
+        <v>60.560901797867572</v>
       </c>
       <c r="H23">
-        <v>59.973073512003523</v>
+        <v>52.846784987563979</v>
       </c>
       <c r="I23">
-        <v>32.752974398465732</v>
+        <v>51.662682663183389</v>
       </c>
       <c r="J23">
-        <v>55.089442768915461</v>
+        <v>67.993664714863669</v>
       </c>
       <c r="K23">
-        <v>17.952393799359559</v>
+        <v>38.90655060338964</v>
       </c>
       <c r="L23">
-        <v>53.065767019567346</v>
+        <v>42.129540510580576</v>
       </c>
       <c r="M23">
-        <v>48.479877426832999</v>
+        <v>37.502153804489865</v>
       </c>
       <c r="N23">
-        <v>95.342791521874872</v>
+        <v>89.259751065350741</v>
       </c>
       <c r="O23">
-        <v>93.255156498933459</v>
+        <v>96.521929362741744</v>
       </c>
       <c r="P23">
-        <v>45.936663233238519</v>
+        <v>40.049461436467311</v>
       </c>
       <c r="Q23">
-        <v>74.913103523916064</v>
+        <v>75.443781807827762</v>
       </c>
       <c r="R23">
-        <v>60.466517336358265</v>
+        <v>72.737672015502724</v>
       </c>
       <c r="S23">
-        <v>58.983703421804741</v>
+        <v>64.85181911629482</v>
       </c>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24">
-        <v>77.133358060568455</v>
+        <v>30.760679966653584</v>
       </c>
       <c r="D24">
-        <v>55.774369750390484</v>
+        <v>39.542963948808229</v>
       </c>
       <c r="E24">
-        <v>53.247988411637131</v>
+        <v>35.63490932224272</v>
       </c>
       <c r="F24">
-        <v>63.65355531565524</v>
+        <v>20.281027446222275</v>
       </c>
       <c r="G24">
-        <v>60.560901797867572</v>
+        <v>25.435478277507539</v>
       </c>
       <c r="H24">
-        <v>52.846784987563979</v>
+        <v>43.651729351962231</v>
       </c>
       <c r="I24">
-        <v>51.662682663183389</v>
+        <v>43.864075275771107</v>
       </c>
       <c r="J24">
-        <v>67.993664714863669</v>
+        <v>60.589198653306347</v>
       </c>
       <c r="K24">
-        <v>38.90655060338964</v>
+        <v>9.3525474094091496</v>
       </c>
       <c r="L24">
-        <v>42.129540510580576</v>
+        <v>77.812835330694497</v>
       </c>
       <c r="M24">
-        <v>37.502153804489865</v>
+        <v>41.98359217754404</v>
       </c>
       <c r="N24">
-        <v>89.259751065350741</v>
+        <v>85.103030378504798</v>
       </c>
       <c r="O24">
-        <v>96.121779447047032</v>
+        <v>99.244533684192689</v>
       </c>
       <c r="P24">
-        <v>40.049461436467311</v>
+        <v>57.196151286072485</v>
       </c>
       <c r="Q24">
-        <v>75.443781807827762</v>
+        <v>72.686502771269261</v>
       </c>
       <c r="R24">
-        <v>72.737672015502724</v>
+        <v>48.175165763548577</v>
       </c>
       <c r="S24">
-        <v>64.85181911629482</v>
+        <v>47.775533604821398</v>
       </c>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C25">
-        <v>30.760679966653584</v>
+        <v>15.530854741663767</v>
       </c>
       <c r="D25">
-        <v>39.542963948808229</v>
+        <v>48.120269854377632</v>
       </c>
       <c r="E25">
-        <v>35.63490932224272</v>
+        <v>39.773433722067146</v>
       </c>
       <c r="F25">
-        <v>20.281027446222275</v>
+        <v>17.081766473581997</v>
       </c>
       <c r="G25">
-        <v>25.435478277507539</v>
+        <v>45.02790770709381</v>
       </c>
       <c r="H25">
-        <v>43.651729351962231</v>
+        <v>41.771970571687191</v>
       </c>
       <c r="I25">
-        <v>43.864075275771107</v>
+        <v>33.118570053647595</v>
       </c>
       <c r="J25">
-        <v>60.589198653306347</v>
+        <v>68.471572326330232</v>
       </c>
       <c r="K25">
-        <v>9.3525474094091496</v>
+        <v>7.5957661226078317</v>
       </c>
       <c r="L25">
-        <v>77.812835330694497</v>
+        <v>13.986515998840332</v>
       </c>
       <c r="M25">
-        <v>41.98359217754404</v>
+        <v>34.094945306110638</v>
       </c>
       <c r="N25">
-        <v>85.103030378504798</v>
+        <v>98.630239276027112</v>
       </c>
       <c r="O25">
-        <v>99.000306133238226</v>
+        <v>97.950381890450387</v>
       </c>
       <c r="P25">
-        <v>57.196151286072485</v>
+        <v>53.607212840695844</v>
       </c>
       <c r="Q25">
-        <v>72.686502771269261</v>
+        <v>65.536346046034652</v>
       </c>
       <c r="R25">
-        <v>48.175165763548577</v>
+        <v>35.611542573841618</v>
       </c>
       <c r="S25">
-        <v>47.775533604821398</v>
+        <v>57.326686550280805</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C26">
-        <v>15.530854741663767</v>
+        <v>52.254716253457296</v>
       </c>
       <c r="D26">
-        <v>48.120269854377632</v>
+        <v>50.916569655008836</v>
       </c>
       <c r="E26">
-        <v>39.773433722067146</v>
+        <v>56.438105737305641</v>
       </c>
       <c r="F26">
-        <v>17.081766473581997</v>
+        <v>62.818996631382078</v>
       </c>
       <c r="G26">
-        <v>45.02790770709381</v>
+        <v>65.19540475941875</v>
       </c>
       <c r="H26">
-        <v>41.771970571687191</v>
+        <v>43.902154934958098</v>
       </c>
       <c r="I26">
-        <v>33.118570053647595</v>
+        <v>51.974899281386996</v>
       </c>
       <c r="J26">
-        <v>68.471572326330232</v>
+        <v>70.694410838506812</v>
       </c>
       <c r="K26">
-        <v>7.5957661226078317</v>
+        <v>29.387637565521118</v>
       </c>
       <c r="L26">
-        <v>13.986515998840332</v>
+        <v>18.143259975272166</v>
       </c>
       <c r="M26">
-        <v>34.094945306110638</v>
+        <v>46.620146253845824</v>
       </c>
       <c r="N26">
-        <v>98.630239276027112</v>
+        <v>97.185493980967749</v>
       </c>
       <c r="O26">
-        <v>97.582051710371985</v>
+        <v>94.785052376750912</v>
       </c>
       <c r="P26">
-        <v>53.607212840695844</v>
+        <v>47.329029255204105</v>
       </c>
       <c r="Q26">
-        <v>65.536346046034652</v>
+        <v>64.430009786792837</v>
       </c>
       <c r="R26">
-        <v>35.611542573841618</v>
+        <v>54.7405867264251</v>
       </c>
       <c r="S26">
-        <v>57.326686550280805</v>
+        <v>54.575957694814541</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C27">
-        <v>52.254716253457296</v>
+        <v>21.048475149518463</v>
       </c>
       <c r="D27">
-        <v>50.916569655008836</v>
+        <v>49.474472066363937</v>
       </c>
       <c r="E27">
-        <v>56.438105737305641</v>
+        <v>35.823687706301975</v>
       </c>
       <c r="F27">
-        <v>62.818996631382078</v>
+        <v>51.351075864208852</v>
       </c>
       <c r="G27">
-        <v>65.19540475941875</v>
+        <v>68.615299548032269</v>
       </c>
       <c r="H27">
-        <v>43.902154934958098</v>
+        <v>58.122774592649897</v>
       </c>
       <c r="I27">
-        <v>51.974899281386996</v>
+        <v>37.364285532271538</v>
       </c>
       <c r="J27">
-        <v>70.694410838506812</v>
+        <v>57.624554386526498</v>
       </c>
       <c r="K27">
-        <v>29.387637565521118</v>
+        <v>22.288240276896261</v>
       </c>
       <c r="L27">
-        <v>18.143259975272166</v>
+        <v>0.17254352569580078</v>
       </c>
       <c r="M27">
-        <v>46.620146253845824</v>
+        <v>50.653136528463492</v>
       </c>
       <c r="N27">
-        <v>97.185493980967749</v>
+        <v>95.456531746611233</v>
       </c>
       <c r="O27">
-        <v>94.4737874070141</v>
+        <v>66.162007957246132</v>
       </c>
       <c r="P27">
-        <v>47.329029255204105</v>
+        <v>55.790837233776948</v>
       </c>
       <c r="Q27">
-        <v>64.430009786792837</v>
+        <v>62.130534963516943</v>
       </c>
       <c r="R27">
-        <v>54.7405867264251</v>
+        <v>49.934755193609142</v>
       </c>
       <c r="S27">
-        <v>54.575957694814541</v>
+        <v>83.408191900489001</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C28">
-        <v>21.048475149518463</v>
+        <v>33.03389791997909</v>
       </c>
       <c r="D28">
-        <v>49.474472066363937</v>
+        <v>40.270694097433179</v>
       </c>
       <c r="E28">
-        <v>35.823687706301975</v>
+        <v>44.556280869983837</v>
       </c>
       <c r="F28">
-        <v>51.351075864208852</v>
+        <v>14.216417549312856</v>
       </c>
       <c r="G28">
-        <v>68.615299548032269</v>
+        <v>44.538302172742448</v>
       </c>
       <c r="H28">
-        <v>58.122774592649897</v>
+        <v>48.010926242881098</v>
       </c>
       <c r="I28">
-        <v>37.364285532271538</v>
+        <v>32.678245745430686</v>
       </c>
       <c r="J28">
-        <v>57.624554386526498</v>
+        <v>54.609150109769487</v>
       </c>
       <c r="K28">
-        <v>22.288240276896261</v>
+        <v>9.3822241909625728</v>
       </c>
       <c r="L28">
-        <v>0.17254352569580078</v>
+        <v>79.122138627817918</v>
       </c>
       <c r="M28">
-        <v>50.653136528463492</v>
+        <v>21.735208302420951</v>
       </c>
       <c r="N28">
-        <v>95.456531746611233</v>
+        <v>83.019031668520583</v>
       </c>
       <c r="O28">
-        <v>64.941458095110548</v>
+        <v>99.314171460227683</v>
       </c>
       <c r="P28">
-        <v>55.790837233776934</v>
+        <v>60.364133685744847</v>
       </c>
       <c r="Q28">
-        <v>62.130534963516943</v>
+        <v>55.316404779464222</v>
       </c>
       <c r="R28">
-        <v>49.934755193609142</v>
+        <v>53.932041713664844</v>
       </c>
       <c r="S28">
-        <v>83.408191900489001</v>
+        <v>42.421296862954172</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29">
-        <v>33.03389791997909</v>
-      </c>
-      <c r="D29">
-        <v>40.270694097433179</v>
-      </c>
-      <c r="E29">
-        <v>44.556280869983837</v>
-      </c>
-      <c r="F29">
-        <v>14.216417549312856</v>
-      </c>
-      <c r="G29">
-        <v>44.538302172742448</v>
-      </c>
-      <c r="H29">
-        <v>48.010926242881098</v>
-      </c>
-      <c r="I29">
-        <v>32.678245745430686</v>
-      </c>
-      <c r="J29">
-        <v>54.609150109769487</v>
-      </c>
-      <c r="K29">
-        <v>9.3822241909625728</v>
-      </c>
-      <c r="L29">
-        <v>79.122138627817918</v>
-      </c>
-      <c r="M29">
-        <v>21.735208302420951</v>
-      </c>
-      <c r="N29">
-        <v>83.019031668520583</v>
-      </c>
-      <c r="O29">
-        <v>99.092858885728504</v>
-      </c>
-      <c r="P29">
-        <v>60.364133685744847</v>
-      </c>
-      <c r="Q29">
-        <v>55.316404779464222</v>
-      </c>
-      <c r="R29">
-        <v>53.932041713664844</v>
-      </c>
-      <c r="S29">
-        <v>42.421296862954172</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="C30">
+        <v>2.6918456358254184</v>
+      </c>
+      <c r="D30">
+        <v>25.077469527439778</v>
+      </c>
+      <c r="E30">
+        <v>38.184651678503215</v>
+      </c>
+      <c r="F30">
+        <v>40.119202784784385</v>
+      </c>
+      <c r="G30">
+        <v>64.902361491003077</v>
+      </c>
+      <c r="H30">
+        <v>38.730317878687899</v>
+      </c>
+      <c r="I30">
+        <v>30.774614678265362</v>
+      </c>
+      <c r="J30">
+        <v>65.135043179253358</v>
+      </c>
+      <c r="K30">
+        <v>9.4182453364499494</v>
+      </c>
+      <c r="L30">
+        <v>27.393385188680302</v>
+      </c>
+      <c r="M30">
+        <v>46.837278253745289</v>
+      </c>
+      <c r="N30">
+        <v>80.495729929807254</v>
+      </c>
+      <c r="O30">
+        <v>96.874410214356629</v>
+      </c>
+      <c r="P30">
+        <v>46.680990860711383</v>
+      </c>
+      <c r="Q30">
+        <v>49.122941728690137</v>
+      </c>
+      <c r="R30">
+        <v>51.89472304840659</v>
+      </c>
+      <c r="S30">
+        <v>60.290235921608009</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C31">
-        <v>2.6918456358254184</v>
+        <v>29.352469612609287</v>
       </c>
       <c r="D31">
-        <v>25.077469527439778</v>
+        <v>45.555625529526537</v>
       </c>
       <c r="E31">
-        <v>38.184651678503215</v>
+        <v>49.993589082709931</v>
       </c>
       <c r="F31">
-        <v>40.119202784784385</v>
+        <v>26.561600711573423</v>
       </c>
       <c r="G31">
-        <v>64.902361491003077</v>
+        <v>58.484498557621656</v>
       </c>
       <c r="H31">
-        <v>38.730317878687899</v>
+        <v>56.486989629215273</v>
       </c>
       <c r="I31">
-        <v>30.774614678265362</v>
+        <v>37.58126638120951</v>
       </c>
       <c r="J31">
-        <v>65.135043179253358</v>
+        <v>61.126684375998636</v>
       </c>
       <c r="K31">
-        <v>9.4182453364499494</v>
+        <v>14.640741852149604</v>
       </c>
       <c r="L31">
-        <v>27.393385188680302</v>
+        <v>22.116614294723718</v>
       </c>
       <c r="M31">
-        <v>46.837278253745289</v>
+        <v>47.961885560250991</v>
       </c>
       <c r="N31">
-        <v>80.495729929807254</v>
+        <v>96.607619923622167</v>
       </c>
       <c r="O31">
-        <v>96.741359560544083</v>
+        <v>89.349635354322587</v>
       </c>
       <c r="P31">
-        <v>46.680990860711383</v>
+        <v>55.790837233776948</v>
       </c>
       <c r="Q31">
-        <v>49.122941728690137</v>
+        <v>74.702446674621513</v>
       </c>
       <c r="R31">
-        <v>51.89472304840659</v>
+        <v>57.083917203269777</v>
       </c>
       <c r="S31">
-        <v>60.290235921608009</v>
+        <v>66.043373839915688</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C32">
-        <v>29.352469612609287</v>
+        <v>38.465695800190282</v>
       </c>
       <c r="D32">
-        <v>45.555625529526537</v>
+        <v>47.57834435639964</v>
       </c>
       <c r="E32">
-        <v>49.993589082709931</v>
+        <v>34.44851824012391</v>
       </c>
       <c r="F32">
-        <v>26.561600711573423</v>
+        <v>10.908814125351531</v>
       </c>
       <c r="G32">
-        <v>58.484498557621656</v>
+        <v>35.000514742111179</v>
       </c>
       <c r="H32">
-        <v>56.486989629215273</v>
+        <v>56.005275868493371</v>
       </c>
       <c r="I32">
-        <v>37.58126638120951</v>
+        <v>39.495893954383909</v>
       </c>
       <c r="J32">
-        <v>61.126684375998636</v>
+        <v>65.190255297792518</v>
       </c>
       <c r="K32">
-        <v>14.640741852149604</v>
+        <v>20.907881139530797</v>
       </c>
       <c r="L32">
-        <v>22.116614294723718</v>
+        <v>75.10425537404879</v>
       </c>
       <c r="M32">
-        <v>47.961885560250991</v>
+        <v>44.297779568925016</v>
       </c>
       <c r="N32">
-        <v>96.607619923622167</v>
+        <v>83.774443602082926</v>
       </c>
       <c r="O32">
-        <v>89.283749265225154</v>
+        <v>99.242716293314146</v>
       </c>
       <c r="P32">
-        <v>55.790837233776934</v>
+        <v>44.270884232662816</v>
       </c>
       <c r="Q32">
-        <v>74.702446674621513</v>
+        <v>76.464101283044272</v>
       </c>
       <c r="R32">
-        <v>57.083917203269777</v>
+        <v>53.575921889175376</v>
       </c>
       <c r="S32">
-        <v>66.043373839915688</v>
+        <v>55.004932784460308</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C33">
-        <v>38.465695800190282</v>
+        <v>69.113556533738574</v>
       </c>
       <c r="D33">
-        <v>47.57834435639964</v>
+        <v>41.684513343460317</v>
       </c>
       <c r="E33">
-        <v>34.44851824012391</v>
+        <v>43.849888378781856</v>
       </c>
       <c r="F33">
-        <v>10.908814125351531</v>
+        <v>28.286993144354067</v>
       </c>
       <c r="G33">
-        <v>35.000514742111179</v>
+        <v>37.418605947515687</v>
       </c>
       <c r="H33">
-        <v>56.005275868493371</v>
+        <v>54.301470927247706</v>
       </c>
       <c r="I33">
-        <v>39.495893954383909</v>
+        <v>44.60566853414948</v>
       </c>
       <c r="J33">
-        <v>65.190255297792518</v>
+        <v>35.829366779089597</v>
       </c>
       <c r="K33">
-        <v>20.907881139530797</v>
+        <v>21.50222936936736</v>
       </c>
       <c r="L33">
-        <v>75.10425537404879</v>
+        <v>82.14509890113078</v>
       </c>
       <c r="M33">
-        <v>44.297779568925016</v>
+        <v>27.927818428854479</v>
       </c>
       <c r="N33">
-        <v>83.774443602082926</v>
+        <v>82.270167240894679</v>
       </c>
       <c r="O33">
-        <v>99.163579670242115</v>
+        <v>73.215767976316329</v>
       </c>
       <c r="P33">
-        <v>44.27088423266283</v>
+        <v>50.908478620939398</v>
       </c>
       <c r="Q33">
-        <v>76.464101283044272</v>
+        <v>65.847292428888693</v>
       </c>
       <c r="R33">
-        <v>53.575921889175376</v>
+        <v>44.765180859296279</v>
       </c>
       <c r="S33">
-        <v>55.004932784460308</v>
+        <v>68.248088064532212</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C34">
-        <v>69.113556533738574</v>
+        <v>84.839250277057474</v>
       </c>
       <c r="D34">
-        <v>41.684513343460317</v>
+        <v>75.067653554516241</v>
       </c>
       <c r="E34">
-        <v>43.849888378781856</v>
+        <v>73.842935557701225</v>
       </c>
       <c r="F34">
-        <v>28.286993144354067</v>
+        <v>82.933434522142633</v>
       </c>
       <c r="G34">
-        <v>37.418605947515687</v>
+        <v>49.947588857987938</v>
       </c>
       <c r="H34">
-        <v>54.301470927247706</v>
+        <v>57.03992786675542</v>
       </c>
       <c r="I34">
-        <v>44.60566853414948</v>
+        <v>67.448175873351843</v>
       </c>
       <c r="J34">
-        <v>35.829366779089597</v>
+        <v>79.846183471693479</v>
       </c>
       <c r="K34">
-        <v>21.50222936936736</v>
+        <v>44.170096535631053</v>
       </c>
       <c r="L34">
-        <v>82.14509890113078</v>
+        <v>50.518633882764355</v>
       </c>
       <c r="M34">
-        <v>27.927818428854479</v>
+        <v>90.795291139835498</v>
       </c>
       <c r="N34">
-        <v>82.270167240894679</v>
+        <v>65.534237615250646</v>
       </c>
       <c r="O34">
-        <v>72.519239714700745</v>
+        <v>67.953809288167719</v>
       </c>
       <c r="P34">
-        <v>50.908478620939398</v>
+        <v>55.277715562455811</v>
       </c>
       <c r="Q34">
-        <v>65.847292428888693</v>
+        <v>23.497405638957176</v>
       </c>
       <c r="R34">
-        <v>44.765180859296279</v>
+        <v>78.769224899378926</v>
       </c>
       <c r="S34">
-        <v>68.248088064532212</v>
+        <v>77.730131099361202</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C35">
-        <v>84.839250277057474</v>
+        <v>83.99306080259008</v>
       </c>
       <c r="D35">
-        <v>75.067653554516241</v>
+        <v>59.120355722115384</v>
       </c>
       <c r="E35">
-        <v>73.842935557701225</v>
+        <v>73.971991924957749</v>
       </c>
       <c r="F35">
-        <v>82.933434522142633</v>
+        <v>66.325385267156278</v>
       </c>
       <c r="G35">
-        <v>49.947588857987938</v>
+        <v>49.747983650600396</v>
       </c>
       <c r="H35">
-        <v>57.03992786675542</v>
+        <v>66.134727794360018</v>
       </c>
       <c r="I35">
-        <v>67.448175873351843</v>
+        <v>51.730660025229852</v>
       </c>
       <c r="J35">
-        <v>79.846183471693479</v>
+        <v>56.839328116606779</v>
       </c>
       <c r="K35">
-        <v>44.170096535631053</v>
+        <v>43.447962745565057</v>
       </c>
       <c r="L35">
-        <v>50.518633882764355</v>
+        <v>47.923815250396729</v>
       </c>
       <c r="M35">
-        <v>90.795291139835498</v>
+        <v>72.558663304337387</v>
       </c>
       <c r="N35">
-        <v>65.534237615250646</v>
+        <v>75.622183931173367</v>
       </c>
       <c r="O35">
-        <v>63.975543111243667</v>
+        <v>92.373967673346655</v>
       </c>
       <c r="P35">
-        <v>55.277715562455811</v>
+        <v>45.397288419946229</v>
       </c>
       <c r="Q35">
-        <v>23.497405638957176</v>
+        <v>74.318948872703331</v>
       </c>
       <c r="R35">
-        <v>78.769224899378926</v>
+        <v>72.755968319118708</v>
       </c>
       <c r="S35">
-        <v>77.730131099361202</v>
+        <v>61.987907864879091</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>83.99306080259008</v>
+        <v>20.418770430143514</v>
       </c>
       <c r="D36">
-        <v>59.120355722115384</v>
+        <v>33.690451214124778</v>
       </c>
       <c r="E36">
-        <v>73.971991924957749</v>
+        <v>37.805852184077075</v>
       </c>
       <c r="F36">
-        <v>66.325385267156278</v>
+        <v>35.617304216167469</v>
       </c>
       <c r="G36">
-        <v>49.747983650600396</v>
+        <v>59.925336614956088</v>
       </c>
       <c r="H36">
-        <v>66.134727794360018</v>
+        <v>41.109769000547736</v>
       </c>
       <c r="I36">
-        <v>51.730660025229852</v>
+        <v>45.770534046310509</v>
       </c>
       <c r="J36">
-        <v>56.839328116606779</v>
+        <v>65.507870429880754</v>
       </c>
       <c r="K36">
-        <v>43.447962745565057</v>
+        <v>19.531605324080225</v>
       </c>
       <c r="L36">
-        <v>47.923815250396729</v>
+        <v>24.600566944605866</v>
       </c>
       <c r="M36">
-        <v>72.558663304337387</v>
+        <v>51.156889507295588</v>
       </c>
       <c r="N36">
-        <v>75.622183931173367</v>
+        <v>91.112039779041538</v>
       </c>
       <c r="O36">
-        <v>90.860918059752024</v>
+        <v>92.154219941575803</v>
       </c>
       <c r="P36">
-        <v>45.397288419946229</v>
+        <v>59.557450293834712</v>
       </c>
       <c r="Q36">
-        <v>74.318948872703331</v>
+        <v>64.784063925165839</v>
       </c>
       <c r="R36">
-        <v>72.755968319118708</v>
+        <v>52.139277970459581</v>
       </c>
       <c r="S36">
-        <v>61.987907864879091</v>
+        <v>79.214448249807631</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C37">
-        <v>20.418770430143514</v>
+        <v>61.403863977318217</v>
       </c>
       <c r="D37">
-        <v>33.690451214124778</v>
+        <v>39.152710957550262</v>
       </c>
       <c r="E37">
-        <v>37.805852184077075</v>
+        <v>51.17756484932503</v>
       </c>
       <c r="F37">
-        <v>35.617304216167469</v>
+        <v>72.277472479769912</v>
       </c>
       <c r="G37">
-        <v>59.925336614956088</v>
+        <v>81.33060290698225</v>
       </c>
       <c r="H37">
-        <v>41.109769000547736</v>
+        <v>58.997681724553942</v>
       </c>
       <c r="I37">
-        <v>45.770534046310509</v>
+        <v>38.288051854144932</v>
       </c>
       <c r="J37">
-        <v>65.507870429880754</v>
+        <v>60.704176368912712</v>
       </c>
       <c r="K37">
-        <v>19.531605324080225</v>
+        <v>37.720439278737487</v>
       </c>
       <c r="L37">
-        <v>24.600566944605866</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>51.156889507295588</v>
+        <v>57.589192373423643</v>
       </c>
       <c r="N37">
-        <v>91.112039779041538</v>
+        <v>77.432091380243406</v>
       </c>
       <c r="O37">
-        <v>91.853089438920932</v>
+        <v>61.122826058428686</v>
       </c>
       <c r="P37">
-        <v>59.557450293834712</v>
+        <v>55.3757677452043</v>
       </c>
       <c r="Q37">
-        <v>64.784063925165839</v>
+        <v>85.573874796832641</v>
       </c>
       <c r="R37">
-        <v>52.139277970459581</v>
+        <v>68.355157613950951</v>
       </c>
       <c r="S37">
-        <v>79.214448249807631</v>
+        <v>64.017529729815408</v>
       </c>
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C38">
-        <v>61.403863977318217</v>
+        <v>35.761403653277569</v>
       </c>
       <c r="D38">
-        <v>39.152710957550262</v>
+        <v>35.779769656240653</v>
       </c>
       <c r="E38">
-        <v>51.17756484932503</v>
+        <v>41.808021649415259</v>
       </c>
       <c r="F38">
-        <v>72.277472479769912</v>
+        <v>7.968457792207797</v>
       </c>
       <c r="G38">
-        <v>81.33060290698225</v>
+        <v>39.141867202962018</v>
       </c>
       <c r="H38">
-        <v>58.997681724553942</v>
+        <v>40.412730854929677</v>
       </c>
       <c r="I38">
-        <v>38.288051854144932</v>
+        <v>38.59475025146979</v>
       </c>
       <c r="J38">
-        <v>60.704176368912712</v>
+        <v>66.178555134074188</v>
       </c>
       <c r="K38">
-        <v>37.720439278737487</v>
+        <v>9.8304263523521325</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>75.878645802887391</v>
       </c>
       <c r="M38">
-        <v>57.589192373423643</v>
+        <v>41.926429495771018</v>
       </c>
       <c r="N38">
-        <v>77.432091380243406</v>
+        <v>86.54531380882085</v>
       </c>
       <c r="O38">
-        <v>59.757314828150385</v>
+        <v>95.12758247231892</v>
       </c>
       <c r="P38">
-        <v>55.3757677452043</v>
+        <v>44.270884232662816</v>
       </c>
       <c r="Q38">
-        <v>85.573874796832641</v>
+        <v>80.856497980165813</v>
       </c>
       <c r="R38">
-        <v>68.355157613950951</v>
+        <v>58.977909128948092</v>
       </c>
       <c r="S38">
-        <v>64.017529729815408</v>
+        <v>56.567437069049561</v>
       </c>
     </row>
     <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C39">
-        <v>35.761403653277569</v>
+        <v>30.322739755988085</v>
       </c>
       <c r="D39">
-        <v>35.779769656240653</v>
+        <v>36.848776784722965</v>
       </c>
       <c r="E39">
-        <v>41.808021649415259</v>
+        <v>30.453371069180449</v>
       </c>
       <c r="F39">
-        <v>7.968457792207797</v>
+        <v>37.217955702136209</v>
       </c>
       <c r="G39">
-        <v>39.141867202962018</v>
+        <v>38.062183690508036</v>
       </c>
       <c r="H39">
-        <v>40.412730854929677</v>
+        <v>53.521653912463179</v>
       </c>
       <c r="I39">
-        <v>38.59475025146979</v>
+        <v>61.3002719623939</v>
       </c>
       <c r="J39">
-        <v>66.178555134074188</v>
+        <v>50.310192989557663</v>
       </c>
       <c r="K39">
-        <v>9.8304263523521325</v>
+        <v>20.944506825894265</v>
       </c>
       <c r="L39">
-        <v>75.878645802887391</v>
+        <v>14.840623560086105</v>
       </c>
       <c r="M39">
-        <v>41.926429495771018</v>
+        <v>24.481092847868496</v>
       </c>
       <c r="N39">
-        <v>86.54531380882085</v>
+        <v>84.122768959335843</v>
       </c>
       <c r="O39">
-        <v>94.942359411710868</v>
+        <v>96.137889140562109</v>
       </c>
       <c r="P39">
-        <v>44.27088423266283</v>
+        <v>40.365658111107145</v>
       </c>
       <c r="Q39">
-        <v>80.856497980165813</v>
+        <v>82.07306722401745</v>
       </c>
       <c r="R39">
-        <v>58.977909128948092</v>
+        <v>50.102460435693182</v>
       </c>
       <c r="S39">
-        <v>56.567437069049561</v>
+        <v>49.031448015261589</v>
       </c>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C40">
-        <v>30.322739755988085</v>
+        <v>44.422068358900617</v>
       </c>
       <c r="D40">
-        <v>36.848776784722965</v>
+        <v>40.495981645878103</v>
       </c>
       <c r="E40">
-        <v>30.453371069180449</v>
+        <v>65.073264503787712</v>
       </c>
       <c r="F40">
-        <v>37.217955702136209</v>
+        <v>50.977906061456409</v>
       </c>
       <c r="G40">
-        <v>38.062183690508036</v>
+        <v>87.412030412984066</v>
       </c>
       <c r="H40">
-        <v>53.521653912463179</v>
+        <v>56.187158782358679</v>
       </c>
       <c r="I40">
-        <v>61.3002719623939</v>
+        <v>44.081778439752114</v>
       </c>
       <c r="J40">
-        <v>50.310192989557663</v>
+        <v>74.964428751872887</v>
       </c>
       <c r="K40">
-        <v>20.944506825894265</v>
+        <v>27.256299218240652</v>
       </c>
       <c r="L40">
-        <v>14.840623560086105</v>
+        <v>13.655500344827143</v>
       </c>
       <c r="M40">
-        <v>24.481092847868496</v>
+        <v>43.93552452274659</v>
       </c>
       <c r="N40">
-        <v>84.122768959335843</v>
+        <v>96.08376938569171</v>
       </c>
       <c r="O40">
-        <v>95.580374307357616</v>
+        <v>98.648642901211218</v>
       </c>
       <c r="P40">
-        <v>40.365658111107145</v>
+        <v>38.618197517357054</v>
       </c>
       <c r="Q40">
-        <v>82.07306722401745</v>
+        <v>71.110392269575172</v>
       </c>
       <c r="R40">
-        <v>50.102460435693182</v>
+        <v>69.987273127365967</v>
       </c>
       <c r="S40">
-        <v>49.031448015261589</v>
+        <v>61.408406103072672</v>
       </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C41">
-        <v>44.422068358900617</v>
+        <v>41.890934123846385</v>
       </c>
       <c r="D41">
-        <v>40.495981645878103</v>
+        <v>61.992467417161606</v>
       </c>
       <c r="E41">
-        <v>65.073264503787712</v>
+        <v>57.77900163453468</v>
       </c>
       <c r="F41">
-        <v>50.977906061456409</v>
+        <v>72.785542230162463</v>
       </c>
       <c r="G41">
-        <v>87.412030412984066</v>
+        <v>55.686648013966021</v>
       </c>
       <c r="H41">
-        <v>56.187158782358679</v>
+        <v>66.610130223564155</v>
       </c>
       <c r="I41">
-        <v>44.081778439752114</v>
+        <v>40.003884856017436</v>
       </c>
       <c r="J41">
-        <v>74.964428751872887</v>
+        <v>58.339610830804816</v>
       </c>
       <c r="K41">
-        <v>27.256299218240652</v>
+        <v>26.956042472797002</v>
       </c>
       <c r="L41">
-        <v>13.655500344827143</v>
+        <v>87.53961267605635</v>
       </c>
       <c r="M41">
-        <v>43.93552452274659</v>
+        <v>56.014297968035144</v>
       </c>
       <c r="N41">
-        <v>96.08376938569171</v>
+        <v>95.461658321631745</v>
       </c>
       <c r="O41">
-        <v>98.574380639583495</v>
+        <v>89.617830191328196</v>
       </c>
       <c r="P41">
-        <v>38.618197517357046</v>
+        <v>64.879625891738669</v>
       </c>
       <c r="Q41">
-        <v>71.110392269575172</v>
+        <v>57.392968817069935</v>
       </c>
       <c r="R41">
-        <v>69.987273127365967</v>
+        <v>70.905375444719212</v>
       </c>
       <c r="S41">
-        <v>61.408406103072672</v>
+        <v>47.450264151130632</v>
       </c>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C42">
-        <v>41.890934123846385</v>
+        <v>37.64785130211461</v>
       </c>
       <c r="D42">
-        <v>61.992467417161606</v>
+        <v>51.126971011844205</v>
       </c>
       <c r="E42">
-        <v>57.77900163453468</v>
+        <v>52.874518236777419</v>
       </c>
       <c r="F42">
-        <v>72.785542230162463</v>
+        <v>30.617949335736661</v>
       </c>
       <c r="G42">
-        <v>55.686648013966021</v>
+        <v>54.226984048304153</v>
       </c>
       <c r="H42">
-        <v>66.610130223564155</v>
+        <v>57.80875093162517</v>
       </c>
       <c r="I42">
-        <v>40.003884856017436</v>
+        <v>50.734846313232282</v>
       </c>
       <c r="J42">
-        <v>58.339610830804816</v>
+        <v>60.733940118718735</v>
       </c>
       <c r="K42">
-        <v>26.956042472797002</v>
+        <v>27.719805454120173</v>
       </c>
       <c r="L42">
-        <v>87.53961267605635</v>
+        <v>45.32241408254059</v>
       </c>
       <c r="M42">
-        <v>56.014297968035144</v>
+        <v>43.787722326437304</v>
       </c>
       <c r="N42">
-        <v>95.461658321631745</v>
+        <v>95.055808936482578</v>
       </c>
       <c r="O42">
-        <v>88.590645032549631</v>
+        <v>94.753704571734531</v>
       </c>
       <c r="P42">
-        <v>64.879625891738669</v>
+        <v>42.858104836962255</v>
       </c>
       <c r="Q42">
-        <v>57.392968817069935</v>
+        <v>74.871479580039221</v>
       </c>
       <c r="R42">
-        <v>70.905375444719212</v>
+        <v>67.78663136574724</v>
       </c>
       <c r="S42">
-        <v>47.450264151130632</v>
+        <v>80.343293023465804</v>
       </c>
     </row>
     <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43">
-        <v>37.64785130211461</v>
-      </c>
-      <c r="D43">
-        <v>51.126971011844205</v>
-      </c>
-      <c r="E43">
-        <v>52.874518236777419</v>
-      </c>
-      <c r="F43">
-        <v>30.617949335736661</v>
-      </c>
-      <c r="G43">
-        <v>54.226984048304153</v>
-      </c>
-      <c r="H43">
-        <v>57.80875093162517</v>
-      </c>
-      <c r="I43">
-        <v>50.734846313232282</v>
-      </c>
-      <c r="J43">
-        <v>60.733940118718735</v>
-      </c>
-      <c r="K43">
-        <v>27.719805454120173</v>
-      </c>
-      <c r="L43">
-        <v>45.32241408254059</v>
-      </c>
-      <c r="M43">
-        <v>43.787722326437304</v>
-      </c>
-      <c r="N43">
-        <v>95.055808936482578</v>
-      </c>
-      <c r="O43">
-        <v>94.312916932935138</v>
-      </c>
-      <c r="P43">
-        <v>42.858104836962255</v>
-      </c>
-      <c r="Q43">
-        <v>74.871479580039221</v>
-      </c>
-      <c r="R43">
-        <v>67.78663136574724</v>
-      </c>
-      <c r="S43">
-        <v>80.343293023465804</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="C44">
+        <v>38.152139592829663</v>
+      </c>
+      <c r="D44">
+        <v>41.678334379106538</v>
+      </c>
+      <c r="E44">
+        <v>31.464677949810365</v>
+      </c>
+      <c r="F44">
+        <v>42.791502935635357</v>
+      </c>
+      <c r="G44">
+        <v>37.199444630240698</v>
+      </c>
+      <c r="H44">
+        <v>38.899084004291886</v>
+      </c>
+      <c r="I44">
+        <v>41.366175785783298</v>
+      </c>
+      <c r="J44">
+        <v>56.495300663949102</v>
+      </c>
+      <c r="K44">
+        <v>9.1086207926978933</v>
+      </c>
+      <c r="L44">
+        <v>70.326102888080428</v>
+      </c>
+      <c r="M44">
+        <v>35.010977893217948</v>
+      </c>
+      <c r="N44">
+        <v>88.366640297642419</v>
+      </c>
+      <c r="O44">
+        <v>98.380966689848847</v>
+      </c>
+      <c r="P44">
+        <v>48.824821538754314</v>
+      </c>
+      <c r="Q44">
+        <v>63.922178890265329</v>
+      </c>
+      <c r="R44">
+        <v>53.1550954643835</v>
+      </c>
+      <c r="S44">
+        <v>50.564296077588658</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C45">
-        <v>38.152139592829663</v>
+        <v>27.5169744124847</v>
       </c>
       <c r="D45">
-        <v>41.678334379106538</v>
+        <v>36.051880826110235</v>
       </c>
       <c r="E45">
-        <v>31.464677949810365</v>
+        <v>26.755596833140171</v>
       </c>
       <c r="F45">
-        <v>42.791502935635357</v>
+        <v>37.273507429196165</v>
       </c>
       <c r="G45">
-        <v>37.199444630240698</v>
+        <v>23.49571971735827</v>
       </c>
       <c r="H45">
-        <v>38.899084004291886</v>
+        <v>27.710658872095379</v>
       </c>
       <c r="I45">
-        <v>41.366175785783298</v>
+        <v>30.804643911938633</v>
       </c>
       <c r="J45">
-        <v>56.495300663949102</v>
+        <v>21.809800447081855</v>
       </c>
       <c r="K45">
-        <v>9.1086207926978933</v>
+        <v>0.26491148634192996</v>
       </c>
       <c r="L45">
-        <v>70.326102888080428</v>
+        <v>39.467587286317851</v>
       </c>
       <c r="M45">
-        <v>35.010977893217948</v>
+        <v>48.557762179646083</v>
       </c>
       <c r="N45">
-        <v>88.366640297642419</v>
+        <v>98.64464892875111</v>
       </c>
       <c r="O45">
-        <v>98.245048837332433</v>
+        <v>90.848985821367066</v>
       </c>
       <c r="P45">
-        <v>48.824821538754314</v>
+        <v>41.037244123492222</v>
       </c>
       <c r="Q45">
-        <v>63.922178890265329</v>
+        <v>58.175833333333323</v>
       </c>
       <c r="R45">
-        <v>53.1550954643835</v>
+        <v>24.44777712948256</v>
       </c>
       <c r="S45">
-        <v>50.564296077588658</v>
+        <v>49.209514314200263</v>
       </c>
     </row>
     <row r="46" spans="1:19">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="C46">
-        <v>27.5169744124847</v>
+        <v>61.096331496526034</v>
       </c>
       <c r="D46">
-        <v>36.051880826110235</v>
+        <v>56.3657615453372</v>
       </c>
       <c r="E46">
-        <v>26.755596833140171</v>
+        <v>51.053318585296537</v>
       </c>
       <c r="F46">
-        <v>37.273507429196172</v>
+        <v>76.427156060779993</v>
       </c>
       <c r="G46">
-        <v>23.49571971735827</v>
+        <v>84.787372710112805</v>
       </c>
       <c r="H46">
-        <v>27.710658872095379</v>
+        <v>66.987943358810256</v>
       </c>
       <c r="I46">
-        <v>30.804643911938633</v>
+        <v>64.426386050486741</v>
       </c>
       <c r="J46">
-        <v>21.809800447081855</v>
+        <v>58.15049475558758</v>
       </c>
       <c r="K46">
-        <v>0.26491148634192996</v>
+        <v>49.6143892818545</v>
       </c>
       <c r="L46">
-        <v>39.467587286317851</v>
+        <v>0</v>
       </c>
       <c r="M46">
-        <v>48.557762179646083</v>
+        <v>58.450889733290211</v>
       </c>
       <c r="N46">
-        <v>98.64464892875111</v>
+        <v>56.192474562619182</v>
       </c>
       <c r="O46">
-        <v>90.800877233726666</v>
+        <v>87.032995141181431</v>
       </c>
       <c r="P46">
-        <v>41.037244123492222</v>
+        <v>56.282334907537461</v>
       </c>
       <c r="Q46">
-        <v>58.175833333333323</v>
+        <v>63.88985690974863</v>
       </c>
       <c r="R46">
-        <v>24.44777712948256</v>
+        <v>59.988292147190265</v>
       </c>
       <c r="S46">
-        <v>49.209514314200263</v>
+        <v>76.611641021395798</v>
       </c>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C47">
-        <v>61.096331496526034</v>
+        <v>1.1223552996666666</v>
       </c>
       <c r="D47">
-        <v>56.3657615453372</v>
+        <v>17.8881584772023</v>
       </c>
       <c r="E47">
-        <v>51.053318585296537</v>
+        <v>24.650119891834692</v>
       </c>
       <c r="F47">
-        <v>76.427156060779993</v>
+        <v>7.6452599388379214</v>
       </c>
       <c r="G47">
-        <v>84.787372710112805</v>
+        <v>43.399144109790292</v>
       </c>
       <c r="H47">
-        <v>66.987943358810256</v>
+        <v>39.357322167329805</v>
       </c>
       <c r="I47">
-        <v>64.426386050486741</v>
+        <v>26.18527041804041</v>
       </c>
       <c r="J47">
-        <v>58.15049475558758</v>
+        <v>43.465408686326455</v>
       </c>
       <c r="K47">
-        <v>49.6143892818545</v>
+        <v>2.9060275390735808</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>21.971141620421072</v>
       </c>
       <c r="M47">
-        <v>58.450889733290211</v>
+        <v>14.416226231338408</v>
       </c>
       <c r="N47">
-        <v>56.192474562619182</v>
+        <v>32.248235294117649</v>
       </c>
       <c r="O47">
-        <v>79.349765422931199</v>
+        <v>72.369252691146187</v>
       </c>
       <c r="P47">
-        <v>56.282334907537461</v>
+        <v>38.618197517357054</v>
       </c>
       <c r="Q47">
-        <v>63.88985690974863</v>
+        <v>71.107789078014164</v>
       </c>
       <c r="R47">
-        <v>59.988292147190265</v>
+        <v>25.015099095698346</v>
       </c>
       <c r="S47">
-        <v>76.611641021395798</v>
+        <v>13.949967050831651</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C48">
-        <v>1.1223552996666666</v>
+        <v>44.408205412722538</v>
       </c>
       <c r="D48">
-        <v>17.8881584772023</v>
+        <v>15.454800230810372</v>
       </c>
       <c r="E48">
-        <v>24.650119891834692</v>
+        <v>48.710200458489012</v>
       </c>
       <c r="F48">
-        <v>7.6452599388379214</v>
+        <v>26.288871919332522</v>
       </c>
       <c r="G48">
-        <v>43.399144109790292</v>
+        <v>30.753736392958551</v>
       </c>
       <c r="H48">
-        <v>39.357322167329805</v>
+        <v>32.9943967760437</v>
       </c>
       <c r="I48">
-        <v>26.18527041804041</v>
+        <v>58.489323025097534</v>
       </c>
       <c r="J48">
-        <v>43.465408686326455</v>
+        <v>39.22185683047455</v>
       </c>
       <c r="K48">
-        <v>2.9060275390735808</v>
+        <v>22.429333190665396</v>
       </c>
       <c r="L48">
-        <v>21.971141620421072</v>
+        <v>65.938465763145771</v>
       </c>
       <c r="M48">
-        <v>14.416226231338408</v>
+        <v>31.005319704503542</v>
       </c>
       <c r="N48">
-        <v>32.248235294117649</v>
+        <v>77.363143758995164</v>
       </c>
       <c r="O48">
-        <v>72.158812295319663</v>
+        <v>98.738269338899528</v>
       </c>
       <c r="P48">
-        <v>38.618197517357046</v>
+        <v>55.02180244365853</v>
       </c>
       <c r="Q48">
-        <v>71.107789078014164</v>
+        <v>75.584987175351984</v>
       </c>
       <c r="R48">
-        <v>25.015099095698346</v>
+        <v>41.424800290847976</v>
       </c>
       <c r="S48">
-        <v>13.949967050831651</v>
+        <v>41.976093991051755</v>
       </c>
     </row>
     <row r="49" spans="1:19">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C49">
-        <v>44.408205412722538</v>
+        <v>42.505793547706567</v>
       </c>
       <c r="D49">
-        <v>15.454800230810372</v>
+        <v>51.35001496993317</v>
       </c>
       <c r="E49">
-        <v>48.710200458489012</v>
+        <v>47.600861428392861</v>
       </c>
       <c r="F49">
-        <v>26.288871919332522</v>
+        <v>55.489767445624615</v>
       </c>
       <c r="G49">
-        <v>30.753736392958551</v>
+        <v>67.415641516136859</v>
       </c>
       <c r="H49">
-        <v>32.9943967760437</v>
+        <v>56.082005554379784</v>
       </c>
       <c r="I49">
-        <v>58.489323025097534</v>
+        <v>60.494537993584082</v>
       </c>
       <c r="J49">
-        <v>39.22185683047455</v>
+        <v>43.100343723833078</v>
       </c>
       <c r="K49">
-        <v>22.429333190665396</v>
+        <v>22.581650414461411</v>
       </c>
       <c r="L49">
-        <v>65.938465763145771</v>
+        <v>0</v>
       </c>
       <c r="M49">
-        <v>31.005319704503542</v>
+        <v>62.009661256175399</v>
       </c>
       <c r="N49">
-        <v>77.363143758995164</v>
+        <v>90.880649533926444</v>
       </c>
       <c r="O49">
-        <v>98.327829551789193</v>
+        <v>52.699200918672119</v>
       </c>
       <c r="P49">
-        <v>55.02180244365853</v>
+        <v>55.790837233776948</v>
       </c>
       <c r="Q49">
-        <v>75.584987175351984</v>
+        <v>63.345406887574399</v>
       </c>
       <c r="R49">
-        <v>41.424800290847976</v>
+        <v>51.460916515610414</v>
       </c>
       <c r="S49">
-        <v>41.976093991051755</v>
+        <v>67.233172079337876</v>
       </c>
     </row>
     <row r="50" spans="1:19">
@@ -3680,7 +3628,7 @@
         <v>88.782011655976078</v>
       </c>
       <c r="O50">
-        <v>98.022257192668263</v>
+        <v>98.215870068841483</v>
       </c>
       <c r="P50">
         <v>52.550824877267317</v>
@@ -3739,7 +3687,7 @@
         <v>95.626828240997455</v>
       </c>
       <c r="O51">
-        <v>98.254513089255354</v>
+        <v>98.616468017709053</v>
       </c>
       <c r="P51">
         <v>28.799549180042806</v>
@@ -3798,7 +3746,7 @@
         <v>74.803416053821849</v>
       </c>
       <c r="O52">
-        <v>88.752940042366205</v>
+        <v>90.704786039773666</v>
       </c>
       <c r="P52">
         <v>56.644794909142021</v>
@@ -3857,10 +3805,10 @@
         <v>84.583799385771925</v>
       </c>
       <c r="O53">
-        <v>98.530587706859606</v>
+        <v>98.64271416893547</v>
       </c>
       <c r="P53">
-        <v>38.618197517357046</v>
+        <v>38.618197517357054</v>
       </c>
       <c r="Q53">
         <v>68.772041252677354</v>
@@ -3916,10 +3864,10 @@
         <v>79.10811795217505</v>
       </c>
       <c r="O54">
-        <v>98.129132894259868</v>
+        <v>98.361193678224566</v>
       </c>
       <c r="P54">
-        <v>55.790837233776934</v>
+        <v>55.790837233776948</v>
       </c>
       <c r="Q54">
         <v>73.862002168748134</v>
@@ -3975,10 +3923,10 @@
         <v>80.180271073795325</v>
       </c>
       <c r="O55">
-        <v>95.528547253033821</v>
+        <v>96.351509564374339</v>
       </c>
       <c r="P55">
-        <v>55.790837233776934</v>
+        <v>55.790837233776948</v>
       </c>
       <c r="Q55">
         <v>77.346516120292407</v>

</xml_diff>